<commit_message>
Gallery Management added and minor fixes
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Excel Files/Club Data/ClubData.xlsx
+++ b/cypress/fixtures/Excel Files/Club Data/ClubData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Automations\cypress\fixtures\Excel Files\Club Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB98D3D4-0990-4E79-8B6E-8A0685AAD274}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75B08E0-0FD4-4EB9-93E7-F6CDC5EC0E3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="144">
   <si>
     <t>clubNameEng</t>
   </si>
@@ -446,6 +446,12 @@
   </si>
   <si>
     <t>09966683987</t>
+  </si>
+  <si>
+    <t>gallery</t>
+  </si>
+  <si>
+    <t>D:/Club Images</t>
   </si>
 </sst>
 </file>
@@ -463,6 +469,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -470,6 +477,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -518,7 +526,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -541,6 +549,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -762,10 +771,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AS79"/>
+  <dimension ref="A1:AT79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA15" sqref="AA15"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AT2" sqref="AT2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -779,7 +788,7 @@
     <col min="27" max="31" width="12.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -915,8 +924,11 @@
       <c r="AS1" s="8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AT1" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>35</v>
       </c>
@@ -1052,8 +1064,9 @@
       <c r="AS2" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AT2" s="14"/>
+    </row>
+    <row r="3" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>95</v>
       </c>
@@ -1190,7 +1203,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>100</v>
       </c>
@@ -1327,7 +1340,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>105</v>
       </c>
@@ -1464,7 +1477,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>110</v>
       </c>
@@ -1601,7 +1614,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>115</v>
       </c>
@@ -1738,7 +1751,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>120</v>
       </c>
@@ -1875,7 +1888,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>125</v>
       </c>
@@ -2011,8 +2024,11 @@
       <c r="AS9" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="10" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AT9" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2037,7 +2053,7 @@
       <c r="V10" s="2"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2062,7 +2078,7 @@
       <c r="V11" s="2"/>
       <c r="W11" s="3"/>
     </row>
-    <row r="12" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2087,7 +2103,7 @@
       <c r="V12" s="2"/>
       <c r="W12" s="3"/>
     </row>
-    <row r="13" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2112,7 +2128,7 @@
       <c r="V13" s="2"/>
       <c r="W13" s="3"/>
     </row>
-    <row r="14" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2137,7 +2153,7 @@
       <c r="V14" s="2"/>
       <c r="W14" s="3"/>
     </row>
-    <row r="15" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2162,7 +2178,7 @@
       <c r="V15" s="2"/>
       <c r="W15" s="3"/>
     </row>
-    <row r="16" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>

<commit_message>
Club Gallery and Logo & banner managed
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Excel Files/Club Data/ClubData.xlsx
+++ b/cypress/fixtures/Excel Files/Club Data/ClubData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Automations\cypress\fixtures\Excel Files\Club Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75B08E0-0FD4-4EB9-93E7-F6CDC5EC0E3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CE69C2-7A45-45DB-AC9A-C1626AC06BB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="144">
   <si>
     <t>clubNameEng</t>
   </si>
@@ -774,7 +774,7 @@
   <dimension ref="A1:AT79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AT2" sqref="AT2"/>
+      <selection activeCell="AK23" sqref="AK23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1064,7 +1064,9 @@
       <c r="AS2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AT2" s="14"/>
+      <c r="AT2" s="14" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="3" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
@@ -1202,6 +1204,9 @@
       <c r="AS3" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="AT3" s="14" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="4" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -1339,6 +1344,9 @@
       <c r="AS4" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="AT4" s="14" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="5" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
@@ -1476,6 +1484,9 @@
       <c r="AS5" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="AT5" s="14" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="6" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
@@ -1613,6 +1624,9 @@
       <c r="AS6" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="AT6" s="14" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="7" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
@@ -1750,6 +1764,9 @@
       <c r="AS7" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="AT7" s="14" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="8" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -1886,6 +1903,9 @@
       </c>
       <c r="AS8" s="2" t="s">
         <v>81</v>
+      </c>
+      <c r="AT8" s="14" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Read me and minor fixes
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Excel Files/Club Data/ClubData.xlsx
+++ b/cypress/fixtures/Excel Files/Club Data/ClubData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Automations\cypress\fixtures\Excel Files\Club Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CE69C2-7A45-45DB-AC9A-C1626AC06BB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CEB28B-71DA-4D93-AB9F-B3E24BE8383D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="142">
   <si>
     <t>clubNameEng</t>
   </si>
@@ -143,12 +143,6 @@
   </si>
   <si>
     <t>clubLogo</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>{{clubNameKatakana}}へようこそ。{{city}}の中心にある最高のホストクラブです。贅沢なエンターテイメントを提供します。{{groupName}}が率いるホストは、素晴らしいサービスを提供します。お問い合わせは{{email}}または{{landlineNumber}}まで。</t>
   </si>
   <si>
     <t>googleMap</t>
@@ -526,7 +520,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -536,9 +530,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -771,10 +762,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AT79"/>
+  <dimension ref="A1:AS79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AK23" sqref="AK23"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -785,10 +776,10 @@
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" style="4"/>
     <col min="21" max="21" width="12.5703125" style="4"/>
-    <col min="27" max="31" width="12.5703125" style="4"/>
+    <col min="26" max="30" width="12.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -864,71 +855,68 @@
       <c r="Y1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AD1" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AE1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="AF1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="AK1" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="AL1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AQ1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AS1" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:46" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AR1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>35</v>
       </c>
@@ -1001,1054 +989,1030 @@
       <c r="X2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Y2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA2" s="13" t="s">
+      <c r="Y2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z2" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK2">
+        <v>5000</v>
+      </c>
+      <c r="AL2">
+        <v>4000</v>
+      </c>
+      <c r="AM2">
+        <v>9000</v>
+      </c>
+      <c r="AN2">
+        <v>5000</v>
+      </c>
+      <c r="AO2">
+        <v>10000</v>
+      </c>
+      <c r="AP2">
+        <v>40</v>
+      </c>
+      <c r="AQ2">
+        <v>25</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1600021</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK3">
+        <v>5000</v>
+      </c>
+      <c r="AL3">
+        <v>4000</v>
+      </c>
+      <c r="AM3">
+        <v>9000</v>
+      </c>
+      <c r="AN3">
+        <v>5000</v>
+      </c>
+      <c r="AO3">
+        <v>10000</v>
+      </c>
+      <c r="AP3">
+        <v>40</v>
+      </c>
+      <c r="AQ3">
+        <v>25</v>
+      </c>
+      <c r="AR3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AS3" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="9">
+        <v>1600022</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z4" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK4">
+        <v>5000</v>
+      </c>
+      <c r="AL4">
+        <v>4000</v>
+      </c>
+      <c r="AM4">
+        <v>9000</v>
+      </c>
+      <c r="AN4">
+        <v>5000</v>
+      </c>
+      <c r="AO4">
+        <v>10000</v>
+      </c>
+      <c r="AP4">
+        <v>40</v>
+      </c>
+      <c r="AQ4">
+        <v>25</v>
+      </c>
+      <c r="AR4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AS4" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="I5" s="9">
+        <v>1600023</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="V5" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z5" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AD5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK5">
+        <v>5000</v>
+      </c>
+      <c r="AL5">
+        <v>4000</v>
+      </c>
+      <c r="AM5">
+        <v>9000</v>
+      </c>
+      <c r="AN5">
+        <v>5000</v>
+      </c>
+      <c r="AO5">
+        <v>10000</v>
+      </c>
+      <c r="AP5">
+        <v>40</v>
+      </c>
+      <c r="AQ5">
+        <v>25</v>
+      </c>
+      <c r="AR5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AS5" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6" s="9">
+        <v>1600024</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="U6" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="V6" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z6" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AA6" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK6">
+        <v>5000</v>
+      </c>
+      <c r="AL6">
+        <v>4000</v>
+      </c>
+      <c r="AM6">
+        <v>9000</v>
+      </c>
+      <c r="AN6">
+        <v>5000</v>
+      </c>
+      <c r="AO6">
+        <v>10000</v>
+      </c>
+      <c r="AP6">
+        <v>40</v>
+      </c>
+      <c r="AQ6">
+        <v>25</v>
+      </c>
+      <c r="AR6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AS6" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="I7" s="9">
+        <v>1600025</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="U7" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="V7" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z7" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA7" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC7" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK7">
+        <v>5000</v>
+      </c>
+      <c r="AL7">
+        <v>4000</v>
+      </c>
+      <c r="AM7">
+        <v>9000</v>
+      </c>
+      <c r="AN7">
+        <v>5000</v>
+      </c>
+      <c r="AO7">
+        <v>10000</v>
+      </c>
+      <c r="AP7">
+        <v>40</v>
+      </c>
+      <c r="AQ7">
+        <v>25</v>
+      </c>
+      <c r="AR7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AS7" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="I8" s="9">
+        <v>1600026</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="U8" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="V8" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z8" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA8" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB8" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD8" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK8">
+        <v>5000</v>
+      </c>
+      <c r="AL8">
+        <v>4000</v>
+      </c>
+      <c r="AM8">
+        <v>9000</v>
+      </c>
+      <c r="AN8">
+        <v>5000</v>
+      </c>
+      <c r="AO8">
+        <v>10000</v>
+      </c>
+      <c r="AP8">
+        <v>40</v>
+      </c>
+      <c r="AQ8">
+        <v>25</v>
+      </c>
+      <c r="AR8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AS8" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="I9" s="9">
+        <v>1600026</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="U9" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="V9" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z9" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC9" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="AC2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AD9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AJ2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL2">
+      <c r="AK9">
         <v>5000</v>
       </c>
-      <c r="AM2">
+      <c r="AL9">
         <v>4000</v>
       </c>
-      <c r="AN2">
+      <c r="AM9">
         <v>9000</v>
       </c>
-      <c r="AO2">
+      <c r="AN9">
         <v>5000</v>
       </c>
-      <c r="AP2">
+      <c r="AO9">
         <v>10000</v>
       </c>
-      <c r="AQ2">
+      <c r="AP9">
         <v>40</v>
       </c>
-      <c r="AR2">
+      <c r="AQ9">
         <v>25</v>
       </c>
-      <c r="AS2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT2" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="I3" s="10">
-        <v>1600021</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="U3" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="V3" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="X3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA3" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB3" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC3" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="AD3" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="AE3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL3">
-        <v>5000</v>
-      </c>
-      <c r="AM3">
-        <v>4000</v>
-      </c>
-      <c r="AN3">
-        <v>9000</v>
-      </c>
-      <c r="AO3">
-        <v>5000</v>
-      </c>
-      <c r="AP3">
-        <v>10000</v>
-      </c>
-      <c r="AQ3">
-        <v>40</v>
-      </c>
-      <c r="AR3">
-        <v>25</v>
-      </c>
-      <c r="AS3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT3" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="I4" s="10">
-        <v>1600022</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="R4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="T4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="V4" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="X4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA4" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="AB4" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC4" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD4" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL4">
-        <v>5000</v>
-      </c>
-      <c r="AM4">
-        <v>4000</v>
-      </c>
-      <c r="AN4">
-        <v>9000</v>
-      </c>
-      <c r="AO4">
-        <v>5000</v>
-      </c>
-      <c r="AP4">
-        <v>10000</v>
-      </c>
-      <c r="AQ4">
-        <v>40</v>
-      </c>
-      <c r="AR4">
-        <v>25</v>
-      </c>
-      <c r="AS4" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT4" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="I5" s="10">
-        <v>1600023</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="P5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="T5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="U5" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="V5" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="X5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y5" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA5" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB5" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="AC5" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD5" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE5" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL5">
-        <v>5000</v>
-      </c>
-      <c r="AM5">
-        <v>4000</v>
-      </c>
-      <c r="AN5">
-        <v>9000</v>
-      </c>
-      <c r="AO5">
-        <v>5000</v>
-      </c>
-      <c r="AP5">
-        <v>10000</v>
-      </c>
-      <c r="AQ5">
-        <v>40</v>
-      </c>
-      <c r="AR5">
-        <v>25</v>
-      </c>
-      <c r="AS5" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT5" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="I6" s="10">
-        <v>1600024</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="T6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="U6" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="V6" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="X6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA6" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB6" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="AC6" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD6" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE6" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL6">
-        <v>5000</v>
-      </c>
-      <c r="AM6">
-        <v>4000</v>
-      </c>
-      <c r="AN6">
-        <v>9000</v>
-      </c>
-      <c r="AO6">
-        <v>5000</v>
-      </c>
-      <c r="AP6">
-        <v>10000</v>
-      </c>
-      <c r="AQ6">
-        <v>40</v>
-      </c>
-      <c r="AR6">
-        <v>25</v>
-      </c>
-      <c r="AS6" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT6" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="I7" s="10">
-        <v>1600025</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="P7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="R7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="T7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="U7" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="V7" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="X7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA7" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB7" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AC7" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD7" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL7">
-        <v>5000</v>
-      </c>
-      <c r="AM7">
-        <v>4000</v>
-      </c>
-      <c r="AN7">
-        <v>9000</v>
-      </c>
-      <c r="AO7">
-        <v>5000</v>
-      </c>
-      <c r="AP7">
-        <v>10000</v>
-      </c>
-      <c r="AQ7">
-        <v>40</v>
-      </c>
-      <c r="AR7">
-        <v>25</v>
-      </c>
-      <c r="AS7" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT7" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="I8" s="10">
-        <v>1600026</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O8" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="P8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="R8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="T8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="U8" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="V8" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="X8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA8" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB8" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC8" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AD8" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE8" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL8">
-        <v>5000</v>
-      </c>
-      <c r="AM8">
-        <v>4000</v>
-      </c>
-      <c r="AN8">
-        <v>9000</v>
-      </c>
-      <c r="AO8">
-        <v>5000</v>
-      </c>
-      <c r="AP8">
-        <v>10000</v>
-      </c>
-      <c r="AQ8">
-        <v>40</v>
-      </c>
-      <c r="AR8">
-        <v>25</v>
-      </c>
-      <c r="AS8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT8" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="I9" s="10">
-        <v>1600026</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="N9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O9" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="P9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="R9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="T9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="U9" s="12" t="s">
+      <c r="AR9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AS9" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="V9" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="X9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA9" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB9" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC9" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE9" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL9">
-        <v>5000</v>
-      </c>
-      <c r="AM9">
-        <v>4000</v>
-      </c>
-      <c r="AN9">
-        <v>9000</v>
-      </c>
-      <c r="AO9">
-        <v>5000</v>
-      </c>
-      <c r="AP9">
-        <v>10000</v>
-      </c>
-      <c r="AQ9">
-        <v>40</v>
-      </c>
-      <c r="AR9">
-        <v>25</v>
-      </c>
-      <c r="AS9" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT9" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2073,7 +2037,7 @@
       <c r="V10" s="2"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2098,7 +2062,7 @@
       <c r="V11" s="2"/>
       <c r="W11" s="3"/>
     </row>
-    <row r="12" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2123,7 +2087,7 @@
       <c r="V12" s="2"/>
       <c r="W12" s="3"/>
     </row>
-    <row r="13" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2148,7 +2112,7 @@
       <c r="V13" s="2"/>
       <c r="W13" s="3"/>
     </row>
-    <row r="14" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2173,7 +2137,7 @@
       <c r="V14" s="2"/>
       <c r="W14" s="3"/>
     </row>
-    <row r="15" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2198,7 +2162,7 @@
       <c r="V15" s="2"/>
       <c r="W15" s="3"/>
     </row>
-    <row r="16" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -3801,77 +3765,77 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="V2" r:id="rId1" display="99HardRockemaill666@gmail.com" xr:uid="{9EE29890-4F75-4E79-B58B-CDD988D2E886}"/>
-    <hyperlink ref="Z2" r:id="rId2" xr:uid="{22D57678-1EAB-4B04-A0D1-C7C6F76E5D90}"/>
-    <hyperlink ref="AF2" r:id="rId3" xr:uid="{30F3C006-E894-4EF5-83B1-2500CCE6A5D2}"/>
-    <hyperlink ref="AG2" r:id="rId4" xr:uid="{311E7B24-7AD4-43B3-97D2-C03BD16B14DD}"/>
-    <hyperlink ref="AH2" r:id="rId5" xr:uid="{462D93DF-C65C-4701-82E1-93D0A5648BB9}"/>
-    <hyperlink ref="AI2" r:id="rId6" xr:uid="{215FD42C-D67B-4D58-ACA7-0FCBF75A9C61}"/>
-    <hyperlink ref="AJ2" r:id="rId7" xr:uid="{2CC482E3-9781-468C-94DB-9CC2FD2DEE2E}"/>
-    <hyperlink ref="AK2" r:id="rId8" xr:uid="{F9E37DC8-F6CE-434E-83D6-FF908103891A}"/>
-    <hyperlink ref="AS2" r:id="rId9" xr:uid="{23D165C6-B605-4D11-B6FC-588FAB8A1298}"/>
+    <hyperlink ref="Y2" r:id="rId2" xr:uid="{22D57678-1EAB-4B04-A0D1-C7C6F76E5D90}"/>
+    <hyperlink ref="AE2" r:id="rId3" xr:uid="{30F3C006-E894-4EF5-83B1-2500CCE6A5D2}"/>
+    <hyperlink ref="AF2" r:id="rId4" xr:uid="{311E7B24-7AD4-43B3-97D2-C03BD16B14DD}"/>
+    <hyperlink ref="AG2" r:id="rId5" xr:uid="{462D93DF-C65C-4701-82E1-93D0A5648BB9}"/>
+    <hyperlink ref="AH2" r:id="rId6" xr:uid="{215FD42C-D67B-4D58-ACA7-0FCBF75A9C61}"/>
+    <hyperlink ref="AI2" r:id="rId7" xr:uid="{2CC482E3-9781-468C-94DB-9CC2FD2DEE2E}"/>
+    <hyperlink ref="AJ2" r:id="rId8" xr:uid="{F9E37DC8-F6CE-434E-83D6-FF908103891A}"/>
+    <hyperlink ref="AR2" r:id="rId9" xr:uid="{23D165C6-B605-4D11-B6FC-588FAB8A1298}"/>
     <hyperlink ref="V6" r:id="rId10" xr:uid="{9359D4E3-CACA-47A7-9CC2-35C4A9AC7D03}"/>
     <hyperlink ref="V4" r:id="rId11" xr:uid="{2A2B5324-C9C7-4AFA-B5D7-48FD15058547}"/>
     <hyperlink ref="V8" r:id="rId12" xr:uid="{1FB40691-6B58-48B8-9D05-503399CBF80A}"/>
     <hyperlink ref="V7" r:id="rId13" xr:uid="{C97A744D-EDBF-4922-9B48-60832D7B4D50}"/>
     <hyperlink ref="V5" r:id="rId14" xr:uid="{AEDCC47E-0D78-42E4-A3D0-83939C740722}"/>
     <hyperlink ref="V3" r:id="rId15" xr:uid="{1A522A4A-13CC-404D-8ECF-B1B35D94E3F5}"/>
-    <hyperlink ref="Z3" r:id="rId16" xr:uid="{4312661F-67D2-4C5E-964D-9639FB9D53DA}"/>
-    <hyperlink ref="Z4" r:id="rId17" xr:uid="{5B16FEBD-409B-4284-AE00-9879F520D173}"/>
-    <hyperlink ref="Z5" r:id="rId18" xr:uid="{7EDEFECD-4A5E-45B8-BB8A-CD0E0946D98F}"/>
-    <hyperlink ref="Z6" r:id="rId19" xr:uid="{21387ACF-3007-4E0D-8F57-CDCA51BE542D}"/>
-    <hyperlink ref="Z7" r:id="rId20" xr:uid="{2C91C5B8-446A-4F98-8FD0-0713A4C7421E}"/>
-    <hyperlink ref="Z8" r:id="rId21" xr:uid="{60BDA731-F231-451C-B1E1-8122B9A07416}"/>
-    <hyperlink ref="AF3" r:id="rId22" xr:uid="{A1D3C90C-7C12-4EC5-A83C-200724407F65}"/>
-    <hyperlink ref="AF4" r:id="rId23" xr:uid="{A95AFEA4-C5FF-4308-864F-8E300FAF0FE9}"/>
-    <hyperlink ref="AF5" r:id="rId24" xr:uid="{22EF5882-90F5-4233-92EC-874E08B74DE9}"/>
-    <hyperlink ref="AF6" r:id="rId25" xr:uid="{16CA8B98-568A-4473-9B70-4CBA5E28AE61}"/>
-    <hyperlink ref="AF7" r:id="rId26" xr:uid="{2AA4F4CB-77E6-42A4-AE0C-FAEB20EB19BA}"/>
-    <hyperlink ref="AF8" r:id="rId27" xr:uid="{0EF0FCE8-C442-4A49-9A70-1C7172BAC725}"/>
-    <hyperlink ref="AF9" r:id="rId28" xr:uid="{70B00255-B7B0-47A6-A3A8-9D8C14A0144C}"/>
-    <hyperlink ref="AG3" r:id="rId29" xr:uid="{B60AE58D-E8A0-4F37-A1DF-8CAE93D8CFBF}"/>
-    <hyperlink ref="AG4" r:id="rId30" xr:uid="{C308F4A6-ED27-41F4-90FD-0073C6EA2DAF}"/>
-    <hyperlink ref="AG5" r:id="rId31" xr:uid="{6694FBAA-7B84-4724-9DDD-CFD621200630}"/>
-    <hyperlink ref="AG6" r:id="rId32" xr:uid="{21F804D6-6090-4119-858A-2E12C2F4E102}"/>
-    <hyperlink ref="AG7" r:id="rId33" xr:uid="{877E1122-AC9E-4DB3-84E0-93A3A4DE8F1E}"/>
-    <hyperlink ref="AG8" r:id="rId34" xr:uid="{139BD8CB-10C3-4CB7-B48E-FAB1D00F19DB}"/>
-    <hyperlink ref="AG9" r:id="rId35" xr:uid="{FC4296D4-304B-4E12-A2BB-91B3E7C9CD1B}"/>
-    <hyperlink ref="AH3" r:id="rId36" xr:uid="{78D38C81-3636-4FDE-B8EB-0DEF2E09B2C0}"/>
-    <hyperlink ref="AH4" r:id="rId37" xr:uid="{B71D0CF8-BF81-49D3-8706-C57B4D26701A}"/>
-    <hyperlink ref="AH5" r:id="rId38" xr:uid="{C54515BC-4766-4E81-ADA3-72E1367E89EB}"/>
-    <hyperlink ref="AH6" r:id="rId39" xr:uid="{11E02B18-0AFF-433F-BCDC-C809D8635B63}"/>
-    <hyperlink ref="AH7" r:id="rId40" xr:uid="{1972EE69-EF2A-4166-8083-F42C884907CD}"/>
-    <hyperlink ref="AH8" r:id="rId41" xr:uid="{86BDAD11-F62C-4882-AED5-275E73419270}"/>
-    <hyperlink ref="AH9" r:id="rId42" xr:uid="{C9AC5D8F-2966-4603-8597-715A0788BD59}"/>
-    <hyperlink ref="AI3" r:id="rId43" xr:uid="{424891AC-4EEB-4E07-ABA9-718B575F42FA}"/>
-    <hyperlink ref="AI4" r:id="rId44" xr:uid="{F27F149B-D5BD-4B9B-9B73-C508F6B18623}"/>
-    <hyperlink ref="AI5" r:id="rId45" xr:uid="{C777DFA5-797D-4A93-9DB5-5682F02B535A}"/>
-    <hyperlink ref="AI6" r:id="rId46" xr:uid="{721E1A15-264F-44DB-AAF2-3D15B2DFDF9C}"/>
-    <hyperlink ref="AI7" r:id="rId47" xr:uid="{156284CF-760F-4820-9507-493220156796}"/>
-    <hyperlink ref="AI8" r:id="rId48" xr:uid="{3B09CF5A-F3A1-47D8-A4C7-95927B938F23}"/>
-    <hyperlink ref="AI9" r:id="rId49" xr:uid="{113F7CF2-18F0-424B-B52B-04D2074B847D}"/>
-    <hyperlink ref="AJ3" r:id="rId50" xr:uid="{58416803-8DF1-4D34-8B80-946D43CBBAEA}"/>
-    <hyperlink ref="AJ4" r:id="rId51" xr:uid="{3349D37C-FD9F-4E1B-81B5-DA20433679B9}"/>
-    <hyperlink ref="AJ5" r:id="rId52" xr:uid="{CB0B1FA9-49C7-4453-B16C-E7EF6919D13C}"/>
-    <hyperlink ref="AJ6" r:id="rId53" xr:uid="{DCC3FF5B-1CD3-42AB-8C71-662185AD31AA}"/>
-    <hyperlink ref="AJ7" r:id="rId54" xr:uid="{BCDCD13D-7DB2-483B-859D-DDBAFECFEDC4}"/>
-    <hyperlink ref="AJ8" r:id="rId55" xr:uid="{C5A2C1FF-DA7C-48F6-ABC6-5CE7398716C2}"/>
-    <hyperlink ref="AJ9" r:id="rId56" xr:uid="{A040E809-93D5-4DB5-8C27-F89FE983F4F7}"/>
-    <hyperlink ref="AK3" r:id="rId57" xr:uid="{B6AA900B-692D-47B2-AD61-D3441CE855D0}"/>
-    <hyperlink ref="AK4" r:id="rId58" xr:uid="{1C584AD9-072D-47B6-9850-2B2B13566F8E}"/>
-    <hyperlink ref="AK5" r:id="rId59" xr:uid="{51A3EEF7-DF23-49EF-A700-A3064AD366F5}"/>
-    <hyperlink ref="AK6" r:id="rId60" xr:uid="{DA530A75-1AA8-4F93-96B2-B20620563DA7}"/>
-    <hyperlink ref="AK7" r:id="rId61" xr:uid="{4E74BD9C-CE85-4027-B8DA-6C5DD385830A}"/>
-    <hyperlink ref="AK8" r:id="rId62" xr:uid="{93ED6EFE-9768-43BD-902F-FF54100E7596}"/>
-    <hyperlink ref="AK9" r:id="rId63" xr:uid="{B80D7872-A434-48F5-AC56-49B4237BEF6F}"/>
-    <hyperlink ref="AS3" r:id="rId64" xr:uid="{F0D560AE-7837-4386-8871-C478BD8B2D15}"/>
-    <hyperlink ref="AS4" r:id="rId65" xr:uid="{0E63DCCD-0B14-453E-8251-1DF937F6C2ED}"/>
-    <hyperlink ref="AS5" r:id="rId66" xr:uid="{40EFF1C6-078A-4D36-9605-3AC4A800C3E9}"/>
-    <hyperlink ref="AS6" r:id="rId67" xr:uid="{F4E12EEC-DB4F-476E-81B8-8C46204F131E}"/>
-    <hyperlink ref="AS7" r:id="rId68" xr:uid="{3BDA4DE9-B4BA-4069-839D-1980F8FDAFD6}"/>
-    <hyperlink ref="AS8" r:id="rId69" xr:uid="{FF2C7332-D737-49DD-B530-0ADAE0CE32CF}"/>
-    <hyperlink ref="AS9" r:id="rId70" xr:uid="{576FCFAA-B3A2-485E-B43D-FAF7551AD9BA}"/>
+    <hyperlink ref="Y3" r:id="rId16" xr:uid="{4312661F-67D2-4C5E-964D-9639FB9D53DA}"/>
+    <hyperlink ref="Y4" r:id="rId17" xr:uid="{5B16FEBD-409B-4284-AE00-9879F520D173}"/>
+    <hyperlink ref="Y5" r:id="rId18" xr:uid="{7EDEFECD-4A5E-45B8-BB8A-CD0E0946D98F}"/>
+    <hyperlink ref="Y6" r:id="rId19" xr:uid="{21387ACF-3007-4E0D-8F57-CDCA51BE542D}"/>
+    <hyperlink ref="Y7" r:id="rId20" xr:uid="{2C91C5B8-446A-4F98-8FD0-0713A4C7421E}"/>
+    <hyperlink ref="Y8" r:id="rId21" xr:uid="{60BDA731-F231-451C-B1E1-8122B9A07416}"/>
+    <hyperlink ref="AE3" r:id="rId22" xr:uid="{A1D3C90C-7C12-4EC5-A83C-200724407F65}"/>
+    <hyperlink ref="AE4" r:id="rId23" xr:uid="{A95AFEA4-C5FF-4308-864F-8E300FAF0FE9}"/>
+    <hyperlink ref="AE5" r:id="rId24" xr:uid="{22EF5882-90F5-4233-92EC-874E08B74DE9}"/>
+    <hyperlink ref="AE6" r:id="rId25" xr:uid="{16CA8B98-568A-4473-9B70-4CBA5E28AE61}"/>
+    <hyperlink ref="AE7" r:id="rId26" xr:uid="{2AA4F4CB-77E6-42A4-AE0C-FAEB20EB19BA}"/>
+    <hyperlink ref="AE8" r:id="rId27" xr:uid="{0EF0FCE8-C442-4A49-9A70-1C7172BAC725}"/>
+    <hyperlink ref="AE9" r:id="rId28" xr:uid="{70B00255-B7B0-47A6-A3A8-9D8C14A0144C}"/>
+    <hyperlink ref="AF3" r:id="rId29" xr:uid="{B60AE58D-E8A0-4F37-A1DF-8CAE93D8CFBF}"/>
+    <hyperlink ref="AF4" r:id="rId30" xr:uid="{C308F4A6-ED27-41F4-90FD-0073C6EA2DAF}"/>
+    <hyperlink ref="AF5" r:id="rId31" xr:uid="{6694FBAA-7B84-4724-9DDD-CFD621200630}"/>
+    <hyperlink ref="AF6" r:id="rId32" xr:uid="{21F804D6-6090-4119-858A-2E12C2F4E102}"/>
+    <hyperlink ref="AF7" r:id="rId33" xr:uid="{877E1122-AC9E-4DB3-84E0-93A3A4DE8F1E}"/>
+    <hyperlink ref="AF8" r:id="rId34" xr:uid="{139BD8CB-10C3-4CB7-B48E-FAB1D00F19DB}"/>
+    <hyperlink ref="AF9" r:id="rId35" xr:uid="{FC4296D4-304B-4E12-A2BB-91B3E7C9CD1B}"/>
+    <hyperlink ref="AG3" r:id="rId36" xr:uid="{78D38C81-3636-4FDE-B8EB-0DEF2E09B2C0}"/>
+    <hyperlink ref="AG4" r:id="rId37" xr:uid="{B71D0CF8-BF81-49D3-8706-C57B4D26701A}"/>
+    <hyperlink ref="AG5" r:id="rId38" xr:uid="{C54515BC-4766-4E81-ADA3-72E1367E89EB}"/>
+    <hyperlink ref="AG6" r:id="rId39" xr:uid="{11E02B18-0AFF-433F-BCDC-C809D8635B63}"/>
+    <hyperlink ref="AG7" r:id="rId40" xr:uid="{1972EE69-EF2A-4166-8083-F42C884907CD}"/>
+    <hyperlink ref="AG8" r:id="rId41" xr:uid="{86BDAD11-F62C-4882-AED5-275E73419270}"/>
+    <hyperlink ref="AG9" r:id="rId42" xr:uid="{C9AC5D8F-2966-4603-8597-715A0788BD59}"/>
+    <hyperlink ref="AH3" r:id="rId43" xr:uid="{424891AC-4EEB-4E07-ABA9-718B575F42FA}"/>
+    <hyperlink ref="AH4" r:id="rId44" xr:uid="{F27F149B-D5BD-4B9B-9B73-C508F6B18623}"/>
+    <hyperlink ref="AH5" r:id="rId45" xr:uid="{C777DFA5-797D-4A93-9DB5-5682F02B535A}"/>
+    <hyperlink ref="AH6" r:id="rId46" xr:uid="{721E1A15-264F-44DB-AAF2-3D15B2DFDF9C}"/>
+    <hyperlink ref="AH7" r:id="rId47" xr:uid="{156284CF-760F-4820-9507-493220156796}"/>
+    <hyperlink ref="AH8" r:id="rId48" xr:uid="{3B09CF5A-F3A1-47D8-A4C7-95927B938F23}"/>
+    <hyperlink ref="AH9" r:id="rId49" xr:uid="{113F7CF2-18F0-424B-B52B-04D2074B847D}"/>
+    <hyperlink ref="AI3" r:id="rId50" xr:uid="{58416803-8DF1-4D34-8B80-946D43CBBAEA}"/>
+    <hyperlink ref="AI4" r:id="rId51" xr:uid="{3349D37C-FD9F-4E1B-81B5-DA20433679B9}"/>
+    <hyperlink ref="AI5" r:id="rId52" xr:uid="{CB0B1FA9-49C7-4453-B16C-E7EF6919D13C}"/>
+    <hyperlink ref="AI6" r:id="rId53" xr:uid="{DCC3FF5B-1CD3-42AB-8C71-662185AD31AA}"/>
+    <hyperlink ref="AI7" r:id="rId54" xr:uid="{BCDCD13D-7DB2-483B-859D-DDBAFECFEDC4}"/>
+    <hyperlink ref="AI8" r:id="rId55" xr:uid="{C5A2C1FF-DA7C-48F6-ABC6-5CE7398716C2}"/>
+    <hyperlink ref="AI9" r:id="rId56" xr:uid="{A040E809-93D5-4DB5-8C27-F89FE983F4F7}"/>
+    <hyperlink ref="AJ3" r:id="rId57" xr:uid="{B6AA900B-692D-47B2-AD61-D3441CE855D0}"/>
+    <hyperlink ref="AJ4" r:id="rId58" xr:uid="{1C584AD9-072D-47B6-9850-2B2B13566F8E}"/>
+    <hyperlink ref="AJ5" r:id="rId59" xr:uid="{51A3EEF7-DF23-49EF-A700-A3064AD366F5}"/>
+    <hyperlink ref="AJ6" r:id="rId60" xr:uid="{DA530A75-1AA8-4F93-96B2-B20620563DA7}"/>
+    <hyperlink ref="AJ7" r:id="rId61" xr:uid="{4E74BD9C-CE85-4027-B8DA-6C5DD385830A}"/>
+    <hyperlink ref="AJ8" r:id="rId62" xr:uid="{93ED6EFE-9768-43BD-902F-FF54100E7596}"/>
+    <hyperlink ref="AJ9" r:id="rId63" xr:uid="{B80D7872-A434-48F5-AC56-49B4237BEF6F}"/>
+    <hyperlink ref="AR3" r:id="rId64" xr:uid="{F0D560AE-7837-4386-8871-C478BD8B2D15}"/>
+    <hyperlink ref="AR4" r:id="rId65" xr:uid="{0E63DCCD-0B14-453E-8251-1DF937F6C2ED}"/>
+    <hyperlink ref="AR5" r:id="rId66" xr:uid="{40EFF1C6-078A-4D36-9605-3AC4A800C3E9}"/>
+    <hyperlink ref="AR6" r:id="rId67" xr:uid="{F4E12EEC-DB4F-476E-81B8-8C46204F131E}"/>
+    <hyperlink ref="AR7" r:id="rId68" xr:uid="{3BDA4DE9-B4BA-4069-839D-1980F8FDAFD6}"/>
+    <hyperlink ref="AR8" r:id="rId69" xr:uid="{FF2C7332-D737-49DD-B530-0ADAE0CE32CF}"/>
+    <hyperlink ref="AR9" r:id="rId70" xr:uid="{576FCFAA-B3A2-485E-B43D-FAF7551AD9BA}"/>
     <hyperlink ref="V9" r:id="rId71" xr:uid="{F191D211-9F11-4D96-947B-D8FDEEB10B11}"/>
-    <hyperlink ref="Z9" r:id="rId72" xr:uid="{9AD55243-CD84-4916-800B-59B1CB29B0BE}"/>
+    <hyperlink ref="Y9" r:id="rId72" xr:uid="{9AD55243-CD84-4916-800B-59B1CB29B0BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId73"/>

</xml_diff>

<commit_message>
Managed Commands folder structure
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Excel Files/Club Data/ClubData.xlsx
+++ b/cypress/fixtures/Excel Files/Club Data/ClubData.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Automations\cypress\fixtures\Excel Files\Club Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CEB28B-71DA-4D93-AB9F-B3E24BE8383D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E80DC7-A819-4655-9BC8-6B8BC9F60EF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="183">
   <si>
     <t>clubNameEng</t>
   </si>
@@ -61,9 +62,6 @@
     <t>kycFileLocation</t>
   </si>
   <si>
-    <t>D:/Web Automations/cypress/fixtures/Files/img1.jpg</t>
-  </si>
-  <si>
     <t>businessFileLocation</t>
   </si>
   <si>
@@ -85,18 +83,12 @@
     <t xml:space="preserve">1丁− 目 </t>
   </si>
   <si>
-    <t>番地号、1</t>
-  </si>
-  <si>
     <t>サーフグループ株式会社</t>
   </si>
   <si>
     <t>新宿区1</t>
   </si>
   <si>
-    <t>山本 花子</t>
-  </si>
-  <si>
     <t>レイスクラブ</t>
   </si>
   <si>
@@ -136,9 +128,6 @@
     <t>99Momentemaill666@gmail.com</t>
   </si>
   <si>
-    <t>09966683981</t>
-  </si>
-  <si>
     <t>clubBanner</t>
   </si>
   <si>
@@ -325,9 +314,6 @@
     <t>Radiance Group</t>
   </si>
   <si>
-    <t>番地号、2</t>
-  </si>
-  <si>
     <t>99RadianceEmail2@gmail.com</t>
   </si>
   <si>
@@ -340,9 +326,6 @@
     <t>Zenith Group</t>
   </si>
   <si>
-    <t>番地号、3</t>
-  </si>
-  <si>
     <t>99ZenithEmail3@gmail.com</t>
   </si>
   <si>
@@ -355,9 +338,6 @@
     <t>Aurora Group</t>
   </si>
   <si>
-    <t>番地号、4</t>
-  </si>
-  <si>
     <t>99AuroraEmail4@gmail.com</t>
   </si>
   <si>
@@ -370,9 +350,6 @@
     <t>Stellar Group</t>
   </si>
   <si>
-    <t>番地号、5</t>
-  </si>
-  <si>
     <t>99StellarEmail5@gmail.com</t>
   </si>
   <si>
@@ -385,9 +362,6 @@
     <t>Nebula Group</t>
   </si>
   <si>
-    <t>番地号、6</t>
-  </si>
-  <si>
     <t>99NebulaEmail6@gmail.com</t>
   </si>
   <si>
@@ -421,38 +395,188 @@
     <t>09012333338</t>
   </si>
   <si>
-    <t>09966683988</t>
-  </si>
-  <si>
-    <t>09966683982</t>
-  </si>
-  <si>
-    <t>09966683983</t>
-  </si>
-  <si>
-    <t>09966683984</t>
-  </si>
-  <si>
-    <t>09966683985</t>
-  </si>
-  <si>
-    <t>09966683986</t>
-  </si>
-  <si>
-    <t>09966683987</t>
-  </si>
-  <si>
     <t>gallery</t>
   </si>
   <si>
     <t>D:/Club Images</t>
+  </si>
+  <si>
+    <t>Elegant Night</t>
+  </si>
+  <si>
+    <t>エレガントナイト</t>
+  </si>
+  <si>
+    <t>Golden Crown</t>
+  </si>
+  <si>
+    <t>ゴールデンクラウン</t>
+  </si>
+  <si>
+    <t>Starlight Hosts</t>
+  </si>
+  <si>
+    <t>スターライトホスト</t>
+  </si>
+  <si>
+    <t>Royal Palace</t>
+  </si>
+  <si>
+    <t>ロイヤルパレス</t>
+  </si>
+  <si>
+    <t>Diamond Lounge</t>
+  </si>
+  <si>
+    <t>ダイヤモンドラウンジ</t>
+  </si>
+  <si>
+    <t>09012333339</t>
+  </si>
+  <si>
+    <t>09012333340</t>
+  </si>
+  <si>
+    <t>09012333341</t>
+  </si>
+  <si>
+    <t>09012333342</t>
+  </si>
+  <si>
+    <t>09012333343</t>
+  </si>
+  <si>
+    <t>新宿区2</t>
+  </si>
+  <si>
+    <t>新宿区3</t>
+  </si>
+  <si>
+    <t>新宿区4</t>
+  </si>
+  <si>
+    <t>新宿区5</t>
+  </si>
+  <si>
+    <t>新宿区6</t>
+  </si>
+  <si>
+    <t>elegant_night@example.com</t>
+  </si>
+  <si>
+    <t>golden_crown@example.com</t>
+  </si>
+  <si>
+    <t>starlight_hosts@example.com</t>
+  </si>
+  <si>
+    <t>royal_palace@example.com</t>
+  </si>
+  <si>
+    <t>diamond_lounge@example.com</t>
+  </si>
+  <si>
+    <t>番地号10</t>
+  </si>
+  <si>
+    <t>番地号1</t>
+  </si>
+  <si>
+    <t>番地号2</t>
+  </si>
+  <si>
+    <t>番地号3</t>
+  </si>
+  <si>
+    <t>番地号4</t>
+  </si>
+  <si>
+    <t>番地号5</t>
+  </si>
+  <si>
+    <t>番地号6</t>
+  </si>
+  <si>
+    <t>番地号7</t>
+  </si>
+  <si>
+    <t>番地号8</t>
+  </si>
+  <si>
+    <t>番地号9</t>
+  </si>
+  <si>
+    <t>番地号11</t>
+  </si>
+  <si>
+    <t>番地号12</t>
+  </si>
+  <si>
+    <t>番地号13</t>
+  </si>
+  <si>
+    <t>09066683981</t>
+  </si>
+  <si>
+    <t>09066683982</t>
+  </si>
+  <si>
+    <t>09066683988</t>
+  </si>
+  <si>
+    <t>09066683986</t>
+  </si>
+  <si>
+    <t>09066683983</t>
+  </si>
+  <si>
+    <t>09066683984</t>
+  </si>
+  <si>
+    <t>09066683985</t>
+  </si>
+  <si>
+    <t>09066683987</t>
+  </si>
+  <si>
+    <t>09066683989</t>
+  </si>
+  <si>
+    <t>09066683990</t>
+  </si>
+  <si>
+    <t>09066683991</t>
+  </si>
+  <si>
+    <t>09066683992</t>
+  </si>
+  <si>
+    <t>09066683999</t>
+  </si>
+  <si>
+    <t>ヤマモト ハナコ</t>
+  </si>
+  <si>
+    <t>D:/Web Automations/cypress/fixtures/Files/kyc.pdf</t>
+  </si>
+  <si>
+    <t>NebulaEmail@example.com</t>
+  </si>
+  <si>
+    <t>Platinum Lounge</t>
+  </si>
+  <si>
+    <t>platinum_lounge@example.com</t>
+  </si>
+  <si>
+    <t>ka1045018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -496,6 +620,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF3E3E3E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -520,7 +659,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -541,6 +680,11 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -762,10 +906,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AS79"/>
+  <dimension ref="A1:AS68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Y24" sqref="Y24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -787,10 +931,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -820,210 +964,210 @@
         <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="U1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="W1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AC1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AD1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="Z1" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AE1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AF1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AG1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AG1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="AK1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AN1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="AR1" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I2" s="1">
         <v>1600021</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>24</v>
+      <c r="N2" t="s">
+        <v>177</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>15</v>
+        <v>178</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>38</v>
+        <v>164</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X2" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Z2" s="12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AB2" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AE2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="AK2">
         <v>5000</v>
@@ -1047,120 +1191,120 @@
         <v>25</v>
       </c>
       <c r="AR2" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="AS2" s="13" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>21</v>
+        <v>92</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="I3" s="9">
         <v>1600021</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="N3" s="9" t="s">
-        <v>24</v>
+        <v>177</v>
       </c>
       <c r="O3" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="V3" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="P3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="U3" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="V3" s="10" t="s">
-        <v>97</v>
-      </c>
       <c r="W3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X3" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AE3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ3" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="AK3">
         <v>5000</v>
@@ -1184,120 +1328,120 @@
         <v>25</v>
       </c>
       <c r="AR3" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="AS3" s="13" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>101</v>
+        <v>92</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="I4" s="9">
         <v>1600022</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="N4" s="9" t="s">
-        <v>24</v>
+        <v>177</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q4" s="9" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="V4" s="10" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Z4" s="12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="AB4" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="AD4" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AE4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AF4" s="2" t="s">
+      <c r="AJ4" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="AK4">
         <v>5000</v>
@@ -1321,120 +1465,120 @@
         <v>25</v>
       </c>
       <c r="AR4" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="AS4" s="13" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>106</v>
+        <v>92</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="I5" s="9">
         <v>1600023</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="N5" s="9" t="s">
-        <v>24</v>
+        <v>177</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5" s="9" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="V5" s="10" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X5" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Z5" s="12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="AB5" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="AC5" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AD5" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AE5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AF5" s="2" t="s">
+      <c r="AJ5" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="AG5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ5" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="AK5">
         <v>5000</v>
@@ -1458,120 +1602,120 @@
         <v>25</v>
       </c>
       <c r="AR5" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="AS5" s="13" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>111</v>
+        <v>92</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="I6" s="9">
         <v>1600024</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M6" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="N6" s="9" t="s">
-        <v>24</v>
+        <v>177</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="V6" s="10" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X6" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Z6" s="12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="AB6" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AC6" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="AD6" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="AE6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AF6" s="2" t="s">
+      <c r="AJ6" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="AG6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ6" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="AK6">
         <v>5000</v>
@@ -1595,120 +1739,120 @@
         <v>25</v>
       </c>
       <c r="AR6" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="AS6" s="13" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>116</v>
+        <v>92</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="I7" s="9">
         <v>1600025</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="N7" s="9" t="s">
-        <v>24</v>
+        <v>177</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S7" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T7" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>137</v>
+        <v>170</v>
       </c>
       <c r="V7" s="10" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X7" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Z7" s="12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="AA7" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="AB7" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="AD7" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AE7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AF7" s="2" t="s">
+      <c r="AJ7" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="AG7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ7" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="AK7">
         <v>5000</v>
@@ -1732,120 +1876,120 @@
         <v>25</v>
       </c>
       <c r="AR7" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="AS7" s="13" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>121</v>
+        <v>92</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="I8" s="9">
         <v>1600026</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>24</v>
+        <v>177</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q8" s="9" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="V8" s="10" t="s">
-        <v>122</v>
+        <v>179</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X8" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Z8" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC8" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD8" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="AA8" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB8" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="AC8" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AD8" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="AE8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AF8" s="2" t="s">
+      <c r="AJ8" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="AG8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ8" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="AK8">
         <v>5000</v>
@@ -1869,120 +2013,120 @@
         <v>25</v>
       </c>
       <c r="AR8" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="AS8" s="13" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>123</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>132</v>
       </c>
       <c r="I9" s="9">
         <v>1600026</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>24</v>
+        <v>177</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q9" s="9" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T9" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="V9" s="10" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X9" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Z9" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="AA9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD9" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="AB9" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="AC9" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD9" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="AE9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AF9" s="2" t="s">
+      <c r="AJ9" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="AG9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ9" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="AK9">
         <v>5000</v>
@@ -2006,161 +2150,833 @@
         <v>25</v>
       </c>
       <c r="AR9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS9" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="I10" s="9">
+        <v>1600026</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="T10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="U10" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z10" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB10" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK10">
+        <v>5000</v>
+      </c>
+      <c r="AL10">
+        <v>4000</v>
+      </c>
+      <c r="AM10">
+        <v>9000</v>
+      </c>
+      <c r="AN10">
+        <v>5000</v>
+      </c>
+      <c r="AO10">
+        <v>10000</v>
+      </c>
+      <c r="AP10">
+        <v>40</v>
+      </c>
+      <c r="AQ10">
+        <v>25</v>
+      </c>
+      <c r="AR10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS10" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="I11" s="9">
+        <v>1600026</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="R11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="T11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="U11" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z11" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA11" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD11" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK11">
+        <v>5000</v>
+      </c>
+      <c r="AL11">
+        <v>4000</v>
+      </c>
+      <c r="AM11">
+        <v>9000</v>
+      </c>
+      <c r="AN11">
+        <v>5000</v>
+      </c>
+      <c r="AO11">
+        <v>10000</v>
+      </c>
+      <c r="AP11">
+        <v>40</v>
+      </c>
+      <c r="AQ11">
+        <v>25</v>
+      </c>
+      <c r="AR11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS11" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="I12" s="9">
+        <v>1600026</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="T12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="U12" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z12" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA12" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC12" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AS9" s="13" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="3"/>
-    </row>
-    <row r="11" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="3"/>
-    </row>
-    <row r="12" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="3"/>
+      <c r="AD12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK12">
+        <v>5000</v>
+      </c>
+      <c r="AL12">
+        <v>4000</v>
+      </c>
+      <c r="AM12">
+        <v>9000</v>
+      </c>
+      <c r="AN12">
+        <v>5000</v>
+      </c>
+      <c r="AO12">
+        <v>10000</v>
+      </c>
+      <c r="AP12">
+        <v>40</v>
+      </c>
+      <c r="AQ12">
+        <v>25</v>
+      </c>
+      <c r="AR12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS12" s="13" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="13" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="3"/>
+      <c r="A13" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I13" s="9">
+        <v>1600026</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="O13" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="T13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="U13" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z13" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC13" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK13">
+        <v>5000</v>
+      </c>
+      <c r="AL13">
+        <v>4000</v>
+      </c>
+      <c r="AM13">
+        <v>9000</v>
+      </c>
+      <c r="AN13">
+        <v>5000</v>
+      </c>
+      <c r="AO13">
+        <v>10000</v>
+      </c>
+      <c r="AP13">
+        <v>40</v>
+      </c>
+      <c r="AQ13">
+        <v>25</v>
+      </c>
+      <c r="AR13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS13" s="13" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="14" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="3"/>
+      <c r="A14" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I14" s="9">
+        <v>1600026</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="R14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="T14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="U14" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z14" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB14" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD14" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK14">
+        <v>5000</v>
+      </c>
+      <c r="AL14">
+        <v>4000</v>
+      </c>
+      <c r="AM14">
+        <v>9000</v>
+      </c>
+      <c r="AN14">
+        <v>5000</v>
+      </c>
+      <c r="AO14">
+        <v>10000</v>
+      </c>
+      <c r="AP14">
+        <v>40</v>
+      </c>
+      <c r="AQ14">
+        <v>25</v>
+      </c>
+      <c r="AR14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS14" s="13" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="15" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="3"/>
+      <c r="A15" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I15" s="9">
+        <v>1600026</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="O15" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="R15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="T15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="U15" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z15" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK15">
+        <v>5000</v>
+      </c>
+      <c r="AL15">
+        <v>4000</v>
+      </c>
+      <c r="AM15">
+        <v>9000</v>
+      </c>
+      <c r="AN15">
+        <v>5000</v>
+      </c>
+      <c r="AO15">
+        <v>10000</v>
+      </c>
+      <c r="AP15">
+        <v>40</v>
+      </c>
+      <c r="AQ15">
+        <v>25</v>
+      </c>
+      <c r="AR15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS15" s="13" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="16" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
@@ -3466,7 +4282,6 @@
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -3487,357 +4302,135 @@
       <c r="V68" s="2"/>
       <c r="W68" s="3"/>
     </row>
-    <row r="69" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="7"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-      <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
-      <c r="S69" s="1"/>
-      <c r="T69" s="1"/>
-      <c r="U69" s="5"/>
-      <c r="V69" s="2"/>
-      <c r="W69" s="3"/>
-    </row>
-    <row r="70" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="7"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
-      <c r="Q70" s="1"/>
-      <c r="R70" s="1"/>
-      <c r="S70" s="1"/>
-      <c r="T70" s="1"/>
-      <c r="U70" s="5"/>
-      <c r="V70" s="2"/>
-      <c r="W70" s="3"/>
-    </row>
-    <row r="71" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="7"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
-      <c r="N71" s="1"/>
-      <c r="O71" s="1"/>
-      <c r="P71" s="1"/>
-      <c r="Q71" s="1"/>
-      <c r="R71" s="1"/>
-      <c r="S71" s="1"/>
-      <c r="T71" s="1"/>
-      <c r="U71" s="5"/>
-      <c r="V71" s="2"/>
-      <c r="W71" s="3"/>
-    </row>
-    <row r="72" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="7"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
-      <c r="M72" s="1"/>
-      <c r="N72" s="1"/>
-      <c r="O72" s="1"/>
-      <c r="P72" s="1"/>
-      <c r="Q72" s="1"/>
-      <c r="R72" s="1"/>
-      <c r="S72" s="1"/>
-      <c r="T72" s="1"/>
-      <c r="U72" s="5"/>
-      <c r="V72" s="2"/>
-      <c r="W72" s="3"/>
-    </row>
-    <row r="73" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="7"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
-      <c r="N73" s="1"/>
-      <c r="O73" s="1"/>
-      <c r="P73" s="1"/>
-      <c r="Q73" s="1"/>
-      <c r="R73" s="1"/>
-      <c r="S73" s="1"/>
-      <c r="T73" s="1"/>
-      <c r="U73" s="5"/>
-      <c r="V73" s="2"/>
-      <c r="W73" s="3"/>
-    </row>
-    <row r="74" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="7"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
-      <c r="N74" s="1"/>
-      <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
-      <c r="R74" s="1"/>
-      <c r="S74" s="1"/>
-      <c r="T74" s="1"/>
-      <c r="U74" s="5"/>
-      <c r="V74" s="2"/>
-      <c r="W74" s="3"/>
-    </row>
-    <row r="75" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="7"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
-      <c r="M75" s="1"/>
-      <c r="N75" s="1"/>
-      <c r="O75" s="1"/>
-      <c r="P75" s="1"/>
-      <c r="Q75" s="1"/>
-      <c r="R75" s="1"/>
-      <c r="S75" s="1"/>
-      <c r="T75" s="1"/>
-      <c r="U75" s="5"/>
-      <c r="V75" s="2"/>
-      <c r="W75" s="3"/>
-    </row>
-    <row r="76" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="7"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-      <c r="L76" s="1"/>
-      <c r="M76" s="1"/>
-      <c r="N76" s="1"/>
-      <c r="O76" s="1"/>
-      <c r="P76" s="1"/>
-      <c r="Q76" s="1"/>
-      <c r="R76" s="1"/>
-      <c r="S76" s="1"/>
-      <c r="T76" s="1"/>
-      <c r="U76" s="5"/>
-      <c r="V76" s="2"/>
-      <c r="W76" s="3"/>
-    </row>
-    <row r="77" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="7"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
-      <c r="M77" s="1"/>
-      <c r="N77" s="1"/>
-      <c r="O77" s="1"/>
-      <c r="P77" s="1"/>
-      <c r="Q77" s="1"/>
-      <c r="R77" s="1"/>
-      <c r="S77" s="1"/>
-      <c r="T77" s="1"/>
-      <c r="U77" s="5"/>
-      <c r="V77" s="2"/>
-      <c r="W77" s="3"/>
-    </row>
-    <row r="78" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="7"/>
-      <c r="I78" s="1"/>
-      <c r="J78" s="1"/>
-      <c r="K78" s="1"/>
-      <c r="L78" s="1"/>
-      <c r="M78" s="1"/>
-      <c r="N78" s="1"/>
-      <c r="O78" s="1"/>
-      <c r="P78" s="1"/>
-      <c r="Q78" s="1"/>
-      <c r="R78" s="1"/>
-      <c r="S78" s="1"/>
-      <c r="T78" s="1"/>
-      <c r="U78" s="5"/>
-      <c r="V78" s="2"/>
-      <c r="W78" s="3"/>
-    </row>
-    <row r="79" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="7"/>
-      <c r="I79" s="1"/>
-      <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
-      <c r="L79" s="1"/>
-      <c r="M79" s="1"/>
-      <c r="N79" s="1"/>
-      <c r="O79" s="1"/>
-      <c r="P79" s="1"/>
-      <c r="Q79" s="1"/>
-      <c r="R79" s="1"/>
-      <c r="S79" s="1"/>
-      <c r="T79" s="1"/>
-      <c r="U79" s="5"/>
-      <c r="V79" s="2"/>
-      <c r="W79" s="3"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="99HardRockemaill666@gmail.com" xr:uid="{9EE29890-4F75-4E79-B58B-CDD988D2E886}"/>
-    <hyperlink ref="Y2" r:id="rId2" xr:uid="{22D57678-1EAB-4B04-A0D1-C7C6F76E5D90}"/>
-    <hyperlink ref="AE2" r:id="rId3" xr:uid="{30F3C006-E894-4EF5-83B1-2500CCE6A5D2}"/>
-    <hyperlink ref="AF2" r:id="rId4" xr:uid="{311E7B24-7AD4-43B3-97D2-C03BD16B14DD}"/>
-    <hyperlink ref="AG2" r:id="rId5" xr:uid="{462D93DF-C65C-4701-82E1-93D0A5648BB9}"/>
-    <hyperlink ref="AH2" r:id="rId6" xr:uid="{215FD42C-D67B-4D58-ACA7-0FCBF75A9C61}"/>
-    <hyperlink ref="AI2" r:id="rId7" xr:uid="{2CC482E3-9781-468C-94DB-9CC2FD2DEE2E}"/>
-    <hyperlink ref="AJ2" r:id="rId8" xr:uid="{F9E37DC8-F6CE-434E-83D6-FF908103891A}"/>
-    <hyperlink ref="AR2" r:id="rId9" xr:uid="{23D165C6-B605-4D11-B6FC-588FAB8A1298}"/>
-    <hyperlink ref="V6" r:id="rId10" xr:uid="{9359D4E3-CACA-47A7-9CC2-35C4A9AC7D03}"/>
-    <hyperlink ref="V4" r:id="rId11" xr:uid="{2A2B5324-C9C7-4AFA-B5D7-48FD15058547}"/>
-    <hyperlink ref="V8" r:id="rId12" xr:uid="{1FB40691-6B58-48B8-9D05-503399CBF80A}"/>
-    <hyperlink ref="V7" r:id="rId13" xr:uid="{C97A744D-EDBF-4922-9B48-60832D7B4D50}"/>
-    <hyperlink ref="V5" r:id="rId14" xr:uid="{AEDCC47E-0D78-42E4-A3D0-83939C740722}"/>
-    <hyperlink ref="V3" r:id="rId15" xr:uid="{1A522A4A-13CC-404D-8ECF-B1B35D94E3F5}"/>
-    <hyperlink ref="Y3" r:id="rId16" xr:uid="{4312661F-67D2-4C5E-964D-9639FB9D53DA}"/>
-    <hyperlink ref="Y4" r:id="rId17" xr:uid="{5B16FEBD-409B-4284-AE00-9879F520D173}"/>
-    <hyperlink ref="Y5" r:id="rId18" xr:uid="{7EDEFECD-4A5E-45B8-BB8A-CD0E0946D98F}"/>
-    <hyperlink ref="Y6" r:id="rId19" xr:uid="{21387ACF-3007-4E0D-8F57-CDCA51BE542D}"/>
-    <hyperlink ref="Y7" r:id="rId20" xr:uid="{2C91C5B8-446A-4F98-8FD0-0713A4C7421E}"/>
-    <hyperlink ref="Y8" r:id="rId21" xr:uid="{60BDA731-F231-451C-B1E1-8122B9A07416}"/>
-    <hyperlink ref="AE3" r:id="rId22" xr:uid="{A1D3C90C-7C12-4EC5-A83C-200724407F65}"/>
-    <hyperlink ref="AE4" r:id="rId23" xr:uid="{A95AFEA4-C5FF-4308-864F-8E300FAF0FE9}"/>
-    <hyperlink ref="AE5" r:id="rId24" xr:uid="{22EF5882-90F5-4233-92EC-874E08B74DE9}"/>
-    <hyperlink ref="AE6" r:id="rId25" xr:uid="{16CA8B98-568A-4473-9B70-4CBA5E28AE61}"/>
-    <hyperlink ref="AE7" r:id="rId26" xr:uid="{2AA4F4CB-77E6-42A4-AE0C-FAEB20EB19BA}"/>
-    <hyperlink ref="AE8" r:id="rId27" xr:uid="{0EF0FCE8-C442-4A49-9A70-1C7172BAC725}"/>
-    <hyperlink ref="AE9" r:id="rId28" xr:uid="{70B00255-B7B0-47A6-A3A8-9D8C14A0144C}"/>
-    <hyperlink ref="AF3" r:id="rId29" xr:uid="{B60AE58D-E8A0-4F37-A1DF-8CAE93D8CFBF}"/>
-    <hyperlink ref="AF4" r:id="rId30" xr:uid="{C308F4A6-ED27-41F4-90FD-0073C6EA2DAF}"/>
-    <hyperlink ref="AF5" r:id="rId31" xr:uid="{6694FBAA-7B84-4724-9DDD-CFD621200630}"/>
-    <hyperlink ref="AF6" r:id="rId32" xr:uid="{21F804D6-6090-4119-858A-2E12C2F4E102}"/>
-    <hyperlink ref="AF7" r:id="rId33" xr:uid="{877E1122-AC9E-4DB3-84E0-93A3A4DE8F1E}"/>
-    <hyperlink ref="AF8" r:id="rId34" xr:uid="{139BD8CB-10C3-4CB7-B48E-FAB1D00F19DB}"/>
-    <hyperlink ref="AF9" r:id="rId35" xr:uid="{FC4296D4-304B-4E12-A2BB-91B3E7C9CD1B}"/>
-    <hyperlink ref="AG3" r:id="rId36" xr:uid="{78D38C81-3636-4FDE-B8EB-0DEF2E09B2C0}"/>
-    <hyperlink ref="AG4" r:id="rId37" xr:uid="{B71D0CF8-BF81-49D3-8706-C57B4D26701A}"/>
-    <hyperlink ref="AG5" r:id="rId38" xr:uid="{C54515BC-4766-4E81-ADA3-72E1367E89EB}"/>
-    <hyperlink ref="AG6" r:id="rId39" xr:uid="{11E02B18-0AFF-433F-BCDC-C809D8635B63}"/>
-    <hyperlink ref="AG7" r:id="rId40" xr:uid="{1972EE69-EF2A-4166-8083-F42C884907CD}"/>
-    <hyperlink ref="AG8" r:id="rId41" xr:uid="{86BDAD11-F62C-4882-AED5-275E73419270}"/>
-    <hyperlink ref="AG9" r:id="rId42" xr:uid="{C9AC5D8F-2966-4603-8597-715A0788BD59}"/>
-    <hyperlink ref="AH3" r:id="rId43" xr:uid="{424891AC-4EEB-4E07-ABA9-718B575F42FA}"/>
-    <hyperlink ref="AH4" r:id="rId44" xr:uid="{F27F149B-D5BD-4B9B-9B73-C508F6B18623}"/>
-    <hyperlink ref="AH5" r:id="rId45" xr:uid="{C777DFA5-797D-4A93-9DB5-5682F02B535A}"/>
-    <hyperlink ref="AH6" r:id="rId46" xr:uid="{721E1A15-264F-44DB-AAF2-3D15B2DFDF9C}"/>
-    <hyperlink ref="AH7" r:id="rId47" xr:uid="{156284CF-760F-4820-9507-493220156796}"/>
-    <hyperlink ref="AH8" r:id="rId48" xr:uid="{3B09CF5A-F3A1-47D8-A4C7-95927B938F23}"/>
-    <hyperlink ref="AH9" r:id="rId49" xr:uid="{113F7CF2-18F0-424B-B52B-04D2074B847D}"/>
-    <hyperlink ref="AI3" r:id="rId50" xr:uid="{58416803-8DF1-4D34-8B80-946D43CBBAEA}"/>
-    <hyperlink ref="AI4" r:id="rId51" xr:uid="{3349D37C-FD9F-4E1B-81B5-DA20433679B9}"/>
-    <hyperlink ref="AI5" r:id="rId52" xr:uid="{CB0B1FA9-49C7-4453-B16C-E7EF6919D13C}"/>
-    <hyperlink ref="AI6" r:id="rId53" xr:uid="{DCC3FF5B-1CD3-42AB-8C71-662185AD31AA}"/>
-    <hyperlink ref="AI7" r:id="rId54" xr:uid="{BCDCD13D-7DB2-483B-859D-DDBAFECFEDC4}"/>
-    <hyperlink ref="AI8" r:id="rId55" xr:uid="{C5A2C1FF-DA7C-48F6-ABC6-5CE7398716C2}"/>
-    <hyperlink ref="AI9" r:id="rId56" xr:uid="{A040E809-93D5-4DB5-8C27-F89FE983F4F7}"/>
-    <hyperlink ref="AJ3" r:id="rId57" xr:uid="{B6AA900B-692D-47B2-AD61-D3441CE855D0}"/>
-    <hyperlink ref="AJ4" r:id="rId58" xr:uid="{1C584AD9-072D-47B6-9850-2B2B13566F8E}"/>
-    <hyperlink ref="AJ5" r:id="rId59" xr:uid="{51A3EEF7-DF23-49EF-A700-A3064AD366F5}"/>
-    <hyperlink ref="AJ6" r:id="rId60" xr:uid="{DA530A75-1AA8-4F93-96B2-B20620563DA7}"/>
-    <hyperlink ref="AJ7" r:id="rId61" xr:uid="{4E74BD9C-CE85-4027-B8DA-6C5DD385830A}"/>
-    <hyperlink ref="AJ8" r:id="rId62" xr:uid="{93ED6EFE-9768-43BD-902F-FF54100E7596}"/>
-    <hyperlink ref="AJ9" r:id="rId63" xr:uid="{B80D7872-A434-48F5-AC56-49B4237BEF6F}"/>
-    <hyperlink ref="AR3" r:id="rId64" xr:uid="{F0D560AE-7837-4386-8871-C478BD8B2D15}"/>
-    <hyperlink ref="AR4" r:id="rId65" xr:uid="{0E63DCCD-0B14-453E-8251-1DF937F6C2ED}"/>
-    <hyperlink ref="AR5" r:id="rId66" xr:uid="{40EFF1C6-078A-4D36-9605-3AC4A800C3E9}"/>
-    <hyperlink ref="AR6" r:id="rId67" xr:uid="{F4E12EEC-DB4F-476E-81B8-8C46204F131E}"/>
-    <hyperlink ref="AR7" r:id="rId68" xr:uid="{3BDA4DE9-B4BA-4069-839D-1980F8FDAFD6}"/>
-    <hyperlink ref="AR8" r:id="rId69" xr:uid="{FF2C7332-D737-49DD-B530-0ADAE0CE32CF}"/>
-    <hyperlink ref="AR9" r:id="rId70" xr:uid="{576FCFAA-B3A2-485E-B43D-FAF7551AD9BA}"/>
-    <hyperlink ref="V9" r:id="rId71" xr:uid="{F191D211-9F11-4D96-947B-D8FDEEB10B11}"/>
-    <hyperlink ref="Y9" r:id="rId72" xr:uid="{9AD55243-CD84-4916-800B-59B1CB29B0BE}"/>
+    <hyperlink ref="AR5" r:id="rId1" xr:uid="{40EFF1C6-078A-4D36-9605-3AC4A800C3E9}"/>
+    <hyperlink ref="AR6" r:id="rId2" xr:uid="{F4E12EEC-DB4F-476E-81B8-8C46204F131E}"/>
+    <hyperlink ref="AR7" r:id="rId3" xr:uid="{3BDA4DE9-B4BA-4069-839D-1980F8FDAFD6}"/>
+    <hyperlink ref="AR8" r:id="rId4" xr:uid="{FF2C7332-D737-49DD-B530-0ADAE0CE32CF}"/>
+    <hyperlink ref="AR9" r:id="rId5" xr:uid="{576FCFAA-B3A2-485E-B43D-FAF7551AD9BA}"/>
+    <hyperlink ref="AR10" r:id="rId6" xr:uid="{8A63D1FA-9E88-4CD9-8207-F4625C37FC10}"/>
+    <hyperlink ref="V10" r:id="rId7" xr:uid="{A3A24461-ACC7-4DAF-B45A-9A24E9FD663F}"/>
+    <hyperlink ref="AJ10" r:id="rId8" xr:uid="{7806DA24-DB34-4AAB-B334-2B21809B409E}"/>
+    <hyperlink ref="AI10" r:id="rId9" xr:uid="{1A398502-040F-4B14-A85C-40C2416212A5}"/>
+    <hyperlink ref="AH10" r:id="rId10" xr:uid="{152B10EE-25AE-4FEE-A3BA-6A36CD0578E7}"/>
+    <hyperlink ref="AG10" r:id="rId11" xr:uid="{A4D32900-D8FF-43F8-BD68-F157AA2CC0A2}"/>
+    <hyperlink ref="AF10" r:id="rId12" xr:uid="{5EE3FA70-0C47-4EAD-AC55-8183CA9D2932}"/>
+    <hyperlink ref="AE10" r:id="rId13" xr:uid="{B21CC387-8226-4F3B-83A6-E82E278186E3}"/>
+    <hyperlink ref="Y10" r:id="rId14" xr:uid="{12D5D795-D933-48B6-ABF2-5BC6ABCD882C}"/>
+    <hyperlink ref="Y9" r:id="rId15" xr:uid="{9AD55243-CD84-4916-800B-59B1CB29B0BE}"/>
+    <hyperlink ref="V9" r:id="rId16" xr:uid="{F191D211-9F11-4D96-947B-D8FDEEB10B11}"/>
+    <hyperlink ref="AJ9" r:id="rId17" xr:uid="{B80D7872-A434-48F5-AC56-49B4237BEF6F}"/>
+    <hyperlink ref="AJ8" r:id="rId18" xr:uid="{93ED6EFE-9768-43BD-902F-FF54100E7596}"/>
+    <hyperlink ref="AJ7" r:id="rId19" xr:uid="{4E74BD9C-CE85-4027-B8DA-6C5DD385830A}"/>
+    <hyperlink ref="AJ6" r:id="rId20" xr:uid="{DA530A75-1AA8-4F93-96B2-B20620563DA7}"/>
+    <hyperlink ref="AJ5" r:id="rId21" xr:uid="{51A3EEF7-DF23-49EF-A700-A3064AD366F5}"/>
+    <hyperlink ref="AI9" r:id="rId22" xr:uid="{A040E809-93D5-4DB5-8C27-F89FE983F4F7}"/>
+    <hyperlink ref="AI8" r:id="rId23" xr:uid="{C5A2C1FF-DA7C-48F6-ABC6-5CE7398716C2}"/>
+    <hyperlink ref="AI7" r:id="rId24" xr:uid="{BCDCD13D-7DB2-483B-859D-DDBAFECFEDC4}"/>
+    <hyperlink ref="AI6" r:id="rId25" xr:uid="{DCC3FF5B-1CD3-42AB-8C71-662185AD31AA}"/>
+    <hyperlink ref="AI5" r:id="rId26" xr:uid="{CB0B1FA9-49C7-4453-B16C-E7EF6919D13C}"/>
+    <hyperlink ref="AH9" r:id="rId27" xr:uid="{113F7CF2-18F0-424B-B52B-04D2074B847D}"/>
+    <hyperlink ref="AH8" r:id="rId28" xr:uid="{3B09CF5A-F3A1-47D8-A4C7-95927B938F23}"/>
+    <hyperlink ref="AH7" r:id="rId29" xr:uid="{156284CF-760F-4820-9507-493220156796}"/>
+    <hyperlink ref="AH6" r:id="rId30" xr:uid="{721E1A15-264F-44DB-AAF2-3D15B2DFDF9C}"/>
+    <hyperlink ref="AH5" r:id="rId31" xr:uid="{C777DFA5-797D-4A93-9DB5-5682F02B535A}"/>
+    <hyperlink ref="AG9" r:id="rId32" xr:uid="{C9AC5D8F-2966-4603-8597-715A0788BD59}"/>
+    <hyperlink ref="AG8" r:id="rId33" xr:uid="{86BDAD11-F62C-4882-AED5-275E73419270}"/>
+    <hyperlink ref="AG7" r:id="rId34" xr:uid="{1972EE69-EF2A-4166-8083-F42C884907CD}"/>
+    <hyperlink ref="AG6" r:id="rId35" xr:uid="{11E02B18-0AFF-433F-BCDC-C809D8635B63}"/>
+    <hyperlink ref="AG5" r:id="rId36" xr:uid="{C54515BC-4766-4E81-ADA3-72E1367E89EB}"/>
+    <hyperlink ref="AF9" r:id="rId37" xr:uid="{FC4296D4-304B-4E12-A2BB-91B3E7C9CD1B}"/>
+    <hyperlink ref="AF8" r:id="rId38" xr:uid="{139BD8CB-10C3-4CB7-B48E-FAB1D00F19DB}"/>
+    <hyperlink ref="AF7" r:id="rId39" xr:uid="{877E1122-AC9E-4DB3-84E0-93A3A4DE8F1E}"/>
+    <hyperlink ref="AF6" r:id="rId40" xr:uid="{21F804D6-6090-4119-858A-2E12C2F4E102}"/>
+    <hyperlink ref="AF5" r:id="rId41" xr:uid="{6694FBAA-7B84-4724-9DDD-CFD621200630}"/>
+    <hyperlink ref="AE9" r:id="rId42" xr:uid="{70B00255-B7B0-47A6-A3A8-9D8C14A0144C}"/>
+    <hyperlink ref="AE8" r:id="rId43" xr:uid="{0EF0FCE8-C442-4A49-9A70-1C7172BAC725}"/>
+    <hyperlink ref="AE7" r:id="rId44" xr:uid="{2AA4F4CB-77E6-42A4-AE0C-FAEB20EB19BA}"/>
+    <hyperlink ref="AE6" r:id="rId45" xr:uid="{16CA8B98-568A-4473-9B70-4CBA5E28AE61}"/>
+    <hyperlink ref="AE5" r:id="rId46" xr:uid="{22EF5882-90F5-4233-92EC-874E08B74DE9}"/>
+    <hyperlink ref="Y8" r:id="rId47" xr:uid="{60BDA731-F231-451C-B1E1-8122B9A07416}"/>
+    <hyperlink ref="Y7" r:id="rId48" xr:uid="{2C91C5B8-446A-4F98-8FD0-0713A4C7421E}"/>
+    <hyperlink ref="Y6" r:id="rId49" xr:uid="{21387ACF-3007-4E0D-8F57-CDCA51BE542D}"/>
+    <hyperlink ref="Y5" r:id="rId50" xr:uid="{7EDEFECD-4A5E-45B8-BB8A-CD0E0946D98F}"/>
+    <hyperlink ref="V5" r:id="rId51" xr:uid="{AEDCC47E-0D78-42E4-A3D0-83939C740722}"/>
+    <hyperlink ref="V7" r:id="rId52" xr:uid="{C97A744D-EDBF-4922-9B48-60832D7B4D50}"/>
+    <hyperlink ref="V8" r:id="rId53" xr:uid="{1FB40691-6B58-48B8-9D05-503399CBF80A}"/>
+    <hyperlink ref="V6" r:id="rId54" xr:uid="{9359D4E3-CACA-47A7-9CC2-35C4A9AC7D03}"/>
+    <hyperlink ref="Y11" r:id="rId55" xr:uid="{CB1C2690-2D75-4DBE-9AE3-0C753E200F56}"/>
+    <hyperlink ref="Y12" r:id="rId56" xr:uid="{37C3E69C-0A50-4909-91DD-03AECB357267}"/>
+    <hyperlink ref="Y13" r:id="rId57" xr:uid="{D4099858-D816-4AE3-A579-4D18A4E733E3}"/>
+    <hyperlink ref="Y14" r:id="rId58" xr:uid="{57A21C4B-0CF4-495E-A701-C0EFFF20F58B}"/>
+    <hyperlink ref="AE11" r:id="rId59" xr:uid="{115E8B96-4499-4621-832F-F38B5FF5F1E5}"/>
+    <hyperlink ref="AE12" r:id="rId60" xr:uid="{374F3E00-9B08-4A7F-8C61-A1776D678E7A}"/>
+    <hyperlink ref="AE13" r:id="rId61" xr:uid="{ADDE819E-6C94-4005-9713-BC437CAE04C1}"/>
+    <hyperlink ref="AE14" r:id="rId62" xr:uid="{5F681696-253B-4718-800A-3F74B6B0ABBF}"/>
+    <hyperlink ref="AF11" r:id="rId63" xr:uid="{FA08CD03-87BC-4138-9DBC-679587925954}"/>
+    <hyperlink ref="AF12" r:id="rId64" xr:uid="{CA1C58CB-00C8-4C46-8D69-32CB4AAA06EE}"/>
+    <hyperlink ref="AF13" r:id="rId65" xr:uid="{743880BA-6282-461E-A730-E45D69C53182}"/>
+    <hyperlink ref="AF14" r:id="rId66" xr:uid="{41E4EF80-592D-4693-BB48-3E2863DAEC07}"/>
+    <hyperlink ref="AG11" r:id="rId67" xr:uid="{8F9BE48C-3577-4533-A495-EB27C2F0F9D2}"/>
+    <hyperlink ref="AG12" r:id="rId68" xr:uid="{48751073-92F7-4BDB-97D8-8DD57B1305B0}"/>
+    <hyperlink ref="AG13" r:id="rId69" xr:uid="{EAB95AA8-63AB-4BB7-A5BC-F83D713DE4C0}"/>
+    <hyperlink ref="AG14" r:id="rId70" xr:uid="{D298C582-7E8E-47F9-81FD-D8267B8E84E5}"/>
+    <hyperlink ref="AH11" r:id="rId71" xr:uid="{1616CF63-342A-473F-B3DB-C92F6FDFDE41}"/>
+    <hyperlink ref="AH12" r:id="rId72" xr:uid="{912B94A1-0BA3-4761-A0A3-BC33382FF40E}"/>
+    <hyperlink ref="AH13" r:id="rId73" xr:uid="{A1B38334-4F71-454D-9C1F-4D21B2081935}"/>
+    <hyperlink ref="AH14" r:id="rId74" xr:uid="{01D312EF-3002-4E0D-8150-AD4417144E38}"/>
+    <hyperlink ref="AI11" r:id="rId75" xr:uid="{065EA5C9-070E-44A2-A3D6-EA196030CE09}"/>
+    <hyperlink ref="AI12" r:id="rId76" xr:uid="{585A89D2-7A97-4838-9F50-3FC938B93066}"/>
+    <hyperlink ref="AI13" r:id="rId77" xr:uid="{5E209E9F-AB3B-44C1-AE4F-F7820119EB1A}"/>
+    <hyperlink ref="AI14" r:id="rId78" xr:uid="{4D786F31-42D7-414A-A8F4-EF08D21ECA2B}"/>
+    <hyperlink ref="AJ11" r:id="rId79" xr:uid="{345D63BA-F676-404B-83D2-320AA3499D9D}"/>
+    <hyperlink ref="AJ12" r:id="rId80" xr:uid="{538312FE-27C0-460A-98FA-87709A4164BD}"/>
+    <hyperlink ref="AJ13" r:id="rId81" xr:uid="{2C2BB42E-F01B-43DC-A7E0-75385FFFC520}"/>
+    <hyperlink ref="AJ14" r:id="rId82" xr:uid="{8815FAB7-6936-4EFF-83B9-DDAB3E2AFD1B}"/>
+    <hyperlink ref="V14" r:id="rId83" xr:uid="{133EEFA0-8A05-48F2-A360-0A0A2CC2DFAF}"/>
+    <hyperlink ref="V13" r:id="rId84" xr:uid="{3EE100DD-2920-445A-AD3A-FC74B7956842}"/>
+    <hyperlink ref="V12" r:id="rId85" xr:uid="{6A5CD97A-1C76-4A64-ACD1-5786E57973F4}"/>
+    <hyperlink ref="V11" r:id="rId86" xr:uid="{8EE879DB-D481-4125-BA8E-0444527AE46A}"/>
+    <hyperlink ref="AR14" r:id="rId87" xr:uid="{55E3848A-1F62-4DB8-8B37-2868DE7E7A95}"/>
+    <hyperlink ref="AR13" r:id="rId88" xr:uid="{3E8767B6-ABDC-490A-9F2B-3E7B0002E362}"/>
+    <hyperlink ref="AR12" r:id="rId89" xr:uid="{D4DBFBC5-BD6B-4286-BAE2-72706DF34B9F}"/>
+    <hyperlink ref="AR11" r:id="rId90" xr:uid="{C5FFF16D-E71A-4F7D-AF6B-C8843E820110}"/>
+    <hyperlink ref="Y15" r:id="rId91" xr:uid="{D6C759F7-4857-4FCD-B8C8-E1E403912A04}"/>
+    <hyperlink ref="AE15" r:id="rId92" xr:uid="{6A6B0EE2-D5BD-426D-83C5-19E00240E0D0}"/>
+    <hyperlink ref="AF15" r:id="rId93" xr:uid="{6991F988-FA73-43D3-A065-88F2BA4F5C01}"/>
+    <hyperlink ref="AG15" r:id="rId94" xr:uid="{7CF221DD-64D7-413E-8A85-B06AA57CE967}"/>
+    <hyperlink ref="AH15" r:id="rId95" xr:uid="{D80FFA51-55A3-4E5C-BE08-8E8DD52DFBA8}"/>
+    <hyperlink ref="AI15" r:id="rId96" xr:uid="{FA137C49-940D-4D01-9D4B-5E2537E9AA33}"/>
+    <hyperlink ref="AJ15" r:id="rId97" xr:uid="{77594D71-BD23-4D6B-A72A-EEAA423B741A}"/>
+    <hyperlink ref="V15" r:id="rId98" xr:uid="{C0DA6C11-788F-4923-BAD9-F1EF67DDD445}"/>
+    <hyperlink ref="AR15" r:id="rId99" xr:uid="{8C643867-EC2C-48F6-9187-6B53F1B9CAC0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId73"/>
+  <pageSetup orientation="portrait" r:id="rId100"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3941225-CA91-4B84-ADA8-77E2B762AB05}">
+  <dimension ref="C24:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C24" s="15"/>
+      <c r="E24" t="s">
+        <v>182</v>
+      </c>
+      <c r="F24" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>